<commit_message>
parser werkend en uitgebreider
</commit_message>
<xml_diff>
--- a/logboek Rens.xlsx
+++ b/logboek Rens.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t xml:space="preserve">Logboek</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">09-10-18</t>
   </si>
   <si>
+    <t xml:space="preserve">alleen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Testknop werkend gemaakt</t>
   </si>
   <si>
@@ -56,16 +59,23 @@
   </si>
   <si>
     <t xml:space="preserve">11-10-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parser werkend maar nog niet geïnplementeerd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parser werkend en geïnplementeerd, maar alleen nog de basis foutmeldingen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM"/>
-    <numFmt numFmtId="166" formatCode="HH:MM"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -141,7 +151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,6 +169,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,16 +193,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -233,11 +247,14 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0.5</v>
@@ -247,21 +264,56 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="3" t="n">
         <v>0.458333333333333</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>43385</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>43396</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.53125</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
parser met fout 405 geïnplementeerd
</commit_message>
<xml_diff>
--- a/logboek Rens.xlsx
+++ b/logboek Rens.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t xml:space="preserve">Logboek</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">parser werkend en geïnplementeerd, maar alleen nog de basis foutmeldingen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parser werkend en geïnplementeerd en alle rest-protocollen werken nu(alleen nog niet alle foutmeldingen)</t>
   </si>
 </sst>
 </file>
@@ -193,16 +196,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="90.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -314,7 +317,23 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>43396</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.680555555555556</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
temp en webserver changes
</commit_message>
<xml_diff>
--- a/logboek Rens.xlsx
+++ b/logboek Rens.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t xml:space="preserve">Logboek</t>
   </si>
@@ -68,17 +68,19 @@
   </si>
   <si>
     <t xml:space="preserve">parser werkend en geïnplementeerd en alle rest-protocollen werken nu(alleen nog niet alle foutmeldingen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gateway kan de data van de arduino opvragen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="167" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -154,7 +156,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -172,10 +174,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,10 +194,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,10 +291,10 @@
       <c r="C6" s="4" t="n">
         <v>43385</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="3" t="n">
         <v>0.375</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -310,10 +308,10 @@
       <c r="C7" s="4" t="n">
         <v>43396</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="3" t="n">
         <v>0.53125</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="3" t="n">
         <v>0.625</v>
       </c>
     </row>
@@ -327,14 +325,30 @@
       <c r="C8" s="4" t="n">
         <v>43396</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="3" t="n">
         <v>0.625</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="3" t="n">
         <v>0.680555555555556</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>43398</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.472222222222222</v>
+      </c>
+    </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -403,6 +417,16 @@
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
unittest proberen werkend te krijgen
</commit_message>
<xml_diff>
--- a/logboek Rens.xlsx
+++ b/logboek Rens.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">Logboek</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve">gateway vraagd de data van de arduino op en upload die naar de server elke minuut een keer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bugs gateway oplossen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meerdere arduino’s op de gateway</t>
   </si>
 </sst>
 </file>
@@ -202,10 +208,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -374,9 +380,57 @@
         <v>0.645833333333333</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>43402</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>43403</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>0.666666666666667</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>43404</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.6875</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>